<commit_message>
Fixed diagonal movement logic
</commit_message>
<xml_diff>
--- a/ScrumBoardComplete.xlsx
+++ b/ScrumBoardComplete.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33980" windowHeight="23560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33980" windowHeight="23560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -377,76 +377,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -604,13 +534,13 @@
                   <c:v>0.631578947368421</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.263157894736842</c:v>
+                  <c:v>0.105263157894737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.105263157894737</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0.263157894736842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,7 +945,7 @@
   <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1318,13 +1248,13 @@
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1342,8 +1272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1358,15 +1288,15 @@
       </c>
       <c r="C2" s="1">
         <f>COUNTA(C4:C104)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1">
         <f>COUNTA(D4:D104)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <f>COUNTA(E4:E104)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1">
         <f>SUM(B2:E2)</f>
@@ -1391,7 +1321,7 @@
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -1399,7 +1329,7 @@
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -1407,8 +1337,8 @@
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="C6" s="1" t="s">
-        <v>10</v>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>55</v>
@@ -1471,7 +1401,7 @@
       </c>
     </row>
     <row r="17" spans="2:6">
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1493,7 +1423,7 @@
       </c>
     </row>
     <row r="20" spans="2:6">
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
@@ -1525,7 +1455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1552,11 +1482,11 @@
       </c>
       <c r="C4">
         <f>ScrumBoard!C2</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D6" si="0">C4/$C$7</f>
-        <v>0.26315789473684209</v>
+        <v>0.10526315789473684</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -1566,11 +1496,11 @@
       </c>
       <c r="C5">
         <f>ScrumBoard!D2</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0.10526315789473684</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -1580,11 +1510,11 @@
       </c>
       <c r="C6">
         <f>ScrumBoard!E2</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.26315789473684209</v>
       </c>
     </row>
     <row r="7" spans="2:4">

</xml_diff>

<commit_message>
added standup and updated scrumboard
</commit_message>
<xml_diff>
--- a/ScrumBoardComplete.xlsx
+++ b/ScrumBoardComplete.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33980" windowHeight="23560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33980" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="UserStories" sheetId="1" r:id="rId1"/>
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -242,13 +242,25 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -260,7 +272,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -303,6 +315,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -310,12 +323,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -336,6 +349,7 @@
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="42" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -534,13 +548,13 @@
                   <c:v>0.631578947368421</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0526315789473684</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0526315789473684</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.263157894736842</c:v>
+                  <c:v>0.368421052631579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -944,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A20" activeCellId="2" sqref="A12:XFD12 A17:XFD17 A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -975,45 +989,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:5" s="4" customFormat="1">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:5" s="4" customFormat="1">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:5" s="4" customFormat="1">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1059,17 +1073,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:5" s="4" customFormat="1">
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1087,17 +1101,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:5" s="4" customFormat="1">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1157,17 +1171,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:5" s="4" customFormat="1">
+      <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1199,17 +1213,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="2:5" s="4" customFormat="1">
+      <c r="B20" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1273,7 +1287,7 @@
   <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1288,15 +1302,15 @@
       </c>
       <c r="C2" s="1">
         <f>COUNTA(C4:C104)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1">
         <f>COUNTA(D4:D104)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <f>COUNTA(E4:E104)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1">
         <f>SUM(B2:E2)</f>
@@ -1360,7 +1374,7 @@
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -1373,7 +1387,7 @@
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -1408,14 +1422,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:6" s="4" customFormat="1">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="1" t="s">
@@ -1455,7 +1469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1482,11 +1496,11 @@
       </c>
       <c r="C4">
         <f>ScrumBoard!C2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D6" si="0">C4/$C$7</f>
-        <v>5.2631578947368418E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -1496,11 +1510,11 @@
       </c>
       <c r="C5">
         <f>ScrumBoard!D2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>5.2631578947368418E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -1510,11 +1524,11 @@
       </c>
       <c r="C6">
         <f>ScrumBoard!E2</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>0.26315789473684209</v>
+        <v>0.36842105263157893</v>
       </c>
     </row>
     <row r="7" spans="2:4">

</xml_diff>